<commit_message>
Single cell function complete
</commit_message>
<xml_diff>
--- a/CH-061 Sales per customer.xlsx
+++ b/CH-061 Sales per customer.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{8638EEE2-9350-4970-AF6F-016A378047FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A9B0F0-F6E6-4AA3-9A17-A5453E14141A}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{8638EEE2-9350-4970-AF6F-016A378047FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B00D5E6-7581-492C-ABD4-4C41A4C41256}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!$B$2:$D$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$36</definedName>
     <definedName name="Xref">_xlfn.LAMBDA(_xlpm.v, _xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlpm.v,EDA!$F$3:$F$8,EDA!$G$3:$G$8,"NA"),IF(_xlpm.z="NA",_xlpm.v,Xref(_xlpm.z))))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId3"/>
-    <pivotCache cacheId="26" r:id="rId4"/>
+    <pivotCache cacheId="31" r:id="rId4"/>
+    <pivotCache cacheId="32" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="29">
   <si>
     <t>Result</t>
   </si>
@@ -353,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,22 +400,31 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1087,90 +1098,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D609D59-4633-4F57-90A3-04B986FD1339}" name="PivotTable4" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="P19:Q27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" compact="0" showAll="0" sortType="ascending">
-      <items count="9">
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" showAll="0">
-      <items count="14">
-        <item x="9"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Number" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{330D899A-1282-4F00-8826-4DA467422A57}" name="PivotTable3" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{330D899A-1282-4F00-8826-4DA467422A57}" name="PivotTable3" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="J18:K32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" compact="0" showAll="0">
@@ -1246,6 +1174,89 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Quantity" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D609D59-4633-4F57-90A3-04B986FD1339}" name="PivotTable4" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="P19:Q27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" compact="0" showAll="0" sortType="ascending">
+      <items count="9">
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" showAll="0">
+      <items count="14">
+        <item x="9"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Number" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1536,19 +1547,19 @@
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="I1" s="18" t="s">
+      <c r="G1" s="21"/>
+      <c r="I1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="18"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2057,7 +2068,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C3:C36">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2071,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D72BBC6-7609-4740-9FE7-EFF7EBA1FAAF}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2100,19 +2111,19 @@
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="I1" s="18" t="s">
+      <c r="G1" s="21"/>
+      <c r="I1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="18"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2251,10 +2262,10 @@
       <c r="B7" s="11">
         <v>45138</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="20">
         <v>31</v>
       </c>
       <c r="E7" s="1">
@@ -2278,10 +2289,10 @@
       <c r="B8" s="11">
         <v>45138</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="20">
         <v>35</v>
       </c>
       <c r="E8" s="1">
@@ -2365,10 +2376,10 @@
       <c r="B13" s="11">
         <v>45172</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>36</v>
       </c>
       <c r="E13" s="1"/>
@@ -2377,10 +2388,10 @@
       <c r="B14" s="11">
         <v>45177</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="20">
         <v>28</v>
       </c>
     </row>
@@ -2437,7 +2448,7 @@
       <c r="G18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>2</v>
       </c>
       <c r="K18" t="s">
@@ -2470,7 +2481,7 @@
       <c r="J19" t="s">
         <v>8</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19">
         <v>163</v>
       </c>
       <c r="M19" t="str">
@@ -2481,7 +2492,7 @@
         <f t="array" ref="N19:N32">K19:K32</f>
         <v>163</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="18" t="s">
         <v>26</v>
       </c>
       <c r="Q19" t="s">
@@ -2492,10 +2503,10 @@
       <c r="B20" s="11">
         <v>45220</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="20">
         <v>33</v>
       </c>
       <c r="F20" s="13" t="s">
@@ -2508,7 +2519,7 @@
       <c r="J20" t="s">
         <v>19</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20">
         <v>92</v>
       </c>
       <c r="M20" t="str">
@@ -2521,7 +2532,7 @@
       <c r="P20" t="s">
         <v>7</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q20">
         <v>86</v>
       </c>
       <c r="T20" t="b" cm="1">
@@ -2549,7 +2560,7 @@
       <c r="J21" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21">
         <v>35</v>
       </c>
       <c r="M21" t="str">
@@ -2562,7 +2573,7 @@
       <c r="P21" t="s">
         <v>6</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21">
         <v>11</v>
       </c>
       <c r="T21" t="b">
@@ -2589,7 +2600,7 @@
       <c r="J22" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22">
         <v>13</v>
       </c>
       <c r="M22" t="str">
@@ -2602,7 +2613,7 @@
       <c r="P22" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22">
         <v>52</v>
       </c>
       <c r="T22" t="b">
@@ -2629,7 +2640,7 @@
       <c r="J23" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23">
         <v>135</v>
       </c>
       <c r="M23" t="str">
@@ -2642,7 +2653,7 @@
       <c r="P23" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23">
         <v>92</v>
       </c>
       <c r="T23" t="b">
@@ -2669,7 +2680,7 @@
       <c r="J24" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="20">
+      <c r="K24">
         <v>49</v>
       </c>
       <c r="M24" t="str">
@@ -2682,7 +2693,7 @@
       <c r="P24" t="s">
         <v>20</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24">
         <v>35</v>
       </c>
       <c r="T24" t="b">
@@ -2693,16 +2704,16 @@
       <c r="B25" s="11">
         <v>45246</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="20">
         <v>27</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="20">
+      <c r="K25">
         <v>85</v>
       </c>
       <c r="M25" t="str">
@@ -2715,7 +2726,7 @@
       <c r="P25" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="20">
+      <c r="Q25">
         <v>347</v>
       </c>
       <c r="T25" t="b">
@@ -2735,7 +2746,7 @@
       <c r="J26" t="s">
         <v>4</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26">
         <v>52</v>
       </c>
       <c r="M26" t="str">
@@ -2748,7 +2759,7 @@
       <c r="P26" t="s">
         <v>21</v>
       </c>
-      <c r="Q26" s="20">
+      <c r="Q26">
         <v>114</v>
       </c>
       <c r="T26" t="b">
@@ -2768,7 +2779,7 @@
       <c r="J27" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="20">
+      <c r="K27">
         <v>86</v>
       </c>
       <c r="M27" t="str">
@@ -2781,7 +2792,7 @@
       <c r="P27" t="s">
         <v>22</v>
       </c>
-      <c r="Q27" s="20">
+      <c r="Q27">
         <v>85</v>
       </c>
       <c r="T27" t="b">
@@ -2792,16 +2803,16 @@
       <c r="B28" s="11">
         <v>45276</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="20">
         <v>22</v>
       </c>
       <c r="J28" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K28">
         <v>11</v>
       </c>
       <c r="M28" t="str">
@@ -2816,16 +2827,16 @@
       <c r="B29" s="11">
         <v>45284</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="20">
         <v>34</v>
       </c>
       <c r="J29" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="20">
+      <c r="K29">
         <v>22</v>
       </c>
       <c r="M29" t="str">
@@ -2849,7 +2860,7 @@
       <c r="J30" t="s">
         <v>14</v>
       </c>
-      <c r="K30" s="20">
+      <c r="K30">
         <v>27</v>
       </c>
       <c r="M30" t="str">
@@ -2864,16 +2875,16 @@
       <c r="B31" s="11">
         <v>45292</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="20">
         <v>21</v>
       </c>
       <c r="J31" t="s">
         <v>16</v>
       </c>
-      <c r="K31" s="20">
+      <c r="K31">
         <v>30</v>
       </c>
       <c r="M31" t="str">
@@ -2888,16 +2899,16 @@
       <c r="B32" s="11">
         <v>45301</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="20">
         <v>30</v>
       </c>
       <c r="J32" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="20">
+      <c r="K32">
         <v>22</v>
       </c>
       <c r="M32" t="str">
@@ -2923,10 +2934,10 @@
       <c r="B34" s="11">
         <v>45319</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="20">
         <v>27</v>
       </c>
     </row>
@@ -2934,10 +2945,10 @@
       <c r="B35" s="11">
         <v>45348</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="20">
         <v>23</v>
       </c>
     </row>
@@ -2955,6 +2966,681 @@
     </row>
   </sheetData>
   <autoFilter ref="B2:D36" xr:uid="{8D72BBC6-7609-4740-9FE7-EFF7EBA1FAAF}"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:C36">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$F$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15911667-5F76-4F80-AE54-B8FA01C50CCB}">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="F1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="I1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11">
+        <v>45125</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="16">
+        <v>40</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="11">
+        <v>45126</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="17">
+        <v>22</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="11">
+        <v>45133</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16">
+        <v>24</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="11">
+        <v>45134</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16">
+        <v>12</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="11">
+        <v>45138</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="16">
+        <v>31</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="11">
+        <v>45138</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="16">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="7">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="11">
+        <v>45141</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="I9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="11">
+        <v>45157</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="16">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="I10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="11">
+        <v>45168</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="16">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="11">
+        <v>45169</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="16">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="11">
+        <v>45172</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="16">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="11">
+        <v>45177</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="11">
+        <v>45178</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="11">
+        <v>45183</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="11">
+        <v>45201</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="11">
+        <v>45201</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="16">
+        <v>25</v>
+      </c>
+      <c r="F18" s="4" t="str" cm="1">
+        <f t="array" ref="F18:G26">_xlfn.LET(
+_xlpm.xmap,_xlfn.LAMBDA(_xlpm.v,_xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlpm.v,$F$3:$F$8,$G$3:$G$8,"NA"),IF(_xlpm.z="NA",_xlpm.v,Xref(_xlpm.z)))),
+_xlpm.nID,_xlfn.MAP(F3:F8,_xlfn.LAMBDA(_xlpm.z,IF(ISNUMBER(_xlfn.XMATCH(_xlpm.z,F3:F8)),_xlpm.xmap(_xlpm.z),_xlpm.z))),
+_xlpm.q,_xlfn.HSTACK($F$3:$F$8,_xlpm.nID),
+_xlpm.zz,_xlfn.MAP($C$3:$C$36, _xlfn.LAMBDA(_xlpm.z,_xlfn.XLOOKUP(_xlpm.z,INDEX(_xlpm.q,,1),INDEX(_xlpm.q,,2),_xlpm.z))),
+_xlpm.u, _xlfn.UNIQUE(_xlpm.zz),
+_xlpm.su, _xlfn.SORTBY(_xlpm.u, MATCH(_xlpm.u,{"C-3","C-4","C-8","C-10","C-11","C-13","C-14","C-15"},0)),
+_xlfn.VSTACK({"Customer","Sales"},_xlfn.HSTACK(_xlpm.su,_xlfn.MAP(_xlpm.su,_xlfn.LAMBDA(_xlpm.z,SUM(_xlfn._xlws.FILTER(D3:D36,_xlpm.zz=_xlpm.z))))))
+)</f>
+        <v>Customer</v>
+      </c>
+      <c r="G18" s="5" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="I18" s="4" t="str" cm="1">
+        <f t="array" ref="I18:J26">_xlfn.LET(
+_xlpm.xmap,_xlfn.LAMBDA(_xlpm.v,_xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlpm.v,$F$3:$F$8,$G$3:$G$8,"NA"),IF(_xlpm.z="NA",_xlpm.v,Xref(_xlpm.z)))),
+_xlpm.nID,_xlfn.MAP(F3:F8,_xlfn.LAMBDA(_xlpm.z,IF(ISNUMBER(_xlfn.XMATCH(_xlpm.z,F3:F8)),_xlpm.xmap(_xlpm.z),_xlpm.z))),
+_xlpm.q,_xlfn.HSTACK($F$3:$F$8,_xlpm.nID),
+_xlpm.zz,_xlfn.MAP($C$3:$C$36, _xlfn.LAMBDA(_xlpm.z,_xlfn.XLOOKUP(_xlpm.z,INDEX(_xlpm.q,,1),INDEX(_xlpm.q,,2),_xlpm.z))),
+_xlpm.u, _xlfn.UNIQUE(_xlpm.zz),
+_xlpm.su, _xlfn.SORTBY(_xlpm.u, MATCH(_xlpm.u,"C-"&amp;_xlfn._xlws.SORT(_xlfn.TEXTAFTER(_xlpm.u,"-")+0),0)),
+_xlfn.VSTACK({"Customer","Sales"},_xlfn.HSTACK(_xlpm.su,_xlfn.MAP(_xlpm.su,_xlfn.LAMBDA(_xlpm.z,SUM(_xlfn._xlws.FILTER(D3:D36,_xlpm.zz=_xlpm.z))))))
+)</f>
+        <v>Customer</v>
+      </c>
+      <c r="J18" s="5" t="str">
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="11">
+        <v>45212</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="16">
+        <v>24</v>
+      </c>
+      <c r="F19" s="6" t="str">
+        <v>C-3</v>
+      </c>
+      <c r="G19" s="7">
+        <v>86</v>
+      </c>
+      <c r="I19" s="6" t="str">
+        <v>C-3</v>
+      </c>
+      <c r="J19" s="7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="11">
+        <v>45220</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="16">
+        <v>33</v>
+      </c>
+      <c r="F20" s="6" t="str">
+        <v>C-4</v>
+      </c>
+      <c r="G20" s="7">
+        <v>11</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <v>C-4</v>
+      </c>
+      <c r="J20" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="11">
+        <v>45222</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="16">
+        <v>23</v>
+      </c>
+      <c r="F21" s="6" t="str">
+        <v>C-8</v>
+      </c>
+      <c r="G21" s="9">
+        <v>52</v>
+      </c>
+      <c r="I21" s="6" t="str">
+        <v>C-8</v>
+      </c>
+      <c r="J21" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="11">
+        <v>45222</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="16">
+        <v>37</v>
+      </c>
+      <c r="F22" s="6" t="str">
+        <v>C-10</v>
+      </c>
+      <c r="G22" s="7">
+        <v>92</v>
+      </c>
+      <c r="I22" s="6" t="str">
+        <v>C-10</v>
+      </c>
+      <c r="J22" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="11">
+        <v>45239</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="16">
+        <v>13</v>
+      </c>
+      <c r="F23" s="6" t="str">
+        <v>C-11</v>
+      </c>
+      <c r="G23" s="7">
+        <v>35</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <v>C-11</v>
+      </c>
+      <c r="J23" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="11">
+        <v>45240</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="16">
+        <v>35</v>
+      </c>
+      <c r="F24" s="6" t="str">
+        <v>C-13</v>
+      </c>
+      <c r="G24" s="7">
+        <v>347</v>
+      </c>
+      <c r="I24" s="6" t="str">
+        <v>C-13</v>
+      </c>
+      <c r="J24" s="7">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="11">
+        <v>45246</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="16">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6" t="str">
+        <v>C-14</v>
+      </c>
+      <c r="G25" s="7">
+        <v>114</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <v>C-14</v>
+      </c>
+      <c r="J25" s="7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="11">
+        <v>45262</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="17">
+        <v>30</v>
+      </c>
+      <c r="F26" s="6" t="str">
+        <v>C-15</v>
+      </c>
+      <c r="G26" s="7">
+        <v>85</v>
+      </c>
+      <c r="I26" s="6" t="str">
+        <v>C-15</v>
+      </c>
+      <c r="J26" s="7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="11">
+        <v>45264</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="11">
+        <v>45276</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="11">
+        <v>45284</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="11">
+        <v>45286</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="11">
+        <v>45292</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="11">
+        <v>45301</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="11">
+        <v>45305</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="11">
+        <v>45319</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="11">
+        <v>45348</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="11">
+        <v>45350</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="16">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+  </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:G1"/>
@@ -2966,6 +3652,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up and ready to go
</commit_message>
<xml_diff>
--- a/CH-061 Sales per customer.xlsx
+++ b/CH-061 Sales per customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{8638EEE2-9350-4970-AF6F-016A378047FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B00D5E6-7581-492C-ABD4-4C41A4C41256}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{8638EEE2-9350-4970-AF6F-016A378047FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B886452-49AC-4254-91D0-2EE7B654133C}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,8 +25,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId4"/>
-    <pivotCache cacheId="32" r:id="rId5"/>
+    <pivotCache cacheId="37" r:id="rId4"/>
+    <pivotCache cacheId="38" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1098,7 +1098,90 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{330D899A-1282-4F00-8826-4DA467422A57}" name="PivotTable3" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D609D59-4633-4F57-90A3-04B986FD1339}" name="PivotTable4" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="P19:Q27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" compact="0" showAll="0" sortType="ascending">
+      <items count="9">
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" showAll="0">
+      <items count="14">
+        <item x="9"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Number" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{330D899A-1282-4F00-8826-4DA467422A57}" name="PivotTable3" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="J18:K32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" compact="0" showAll="0">
@@ -1174,89 +1257,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Quantity" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D609D59-4633-4F57-90A3-04B986FD1339}" name="PivotTable4" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="P19:Q27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" compact="0" showAll="0" sortType="ascending">
-      <items count="9">
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" showAll="0">
-      <items count="14">
-        <item x="9"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Number" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2986,7 +2986,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3293,7 +3293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <v>45201</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
         <v>45201</v>
       </c>
@@ -3316,21 +3316,6 @@
       </c>
       <c r="F18" s="4" t="str" cm="1">
         <f t="array" ref="F18:G26">_xlfn.LET(
-_xlpm.xmap,_xlfn.LAMBDA(_xlpm.v,_xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlpm.v,$F$3:$F$8,$G$3:$G$8,"NA"),IF(_xlpm.z="NA",_xlpm.v,Xref(_xlpm.z)))),
-_xlpm.nID,_xlfn.MAP(F3:F8,_xlfn.LAMBDA(_xlpm.z,IF(ISNUMBER(_xlfn.XMATCH(_xlpm.z,F3:F8)),_xlpm.xmap(_xlpm.z),_xlpm.z))),
-_xlpm.q,_xlfn.HSTACK($F$3:$F$8,_xlpm.nID),
-_xlpm.zz,_xlfn.MAP($C$3:$C$36, _xlfn.LAMBDA(_xlpm.z,_xlfn.XLOOKUP(_xlpm.z,INDEX(_xlpm.q,,1),INDEX(_xlpm.q,,2),_xlpm.z))),
-_xlpm.u, _xlfn.UNIQUE(_xlpm.zz),
-_xlpm.su, _xlfn.SORTBY(_xlpm.u, MATCH(_xlpm.u,{"C-3","C-4","C-8","C-10","C-11","C-13","C-14","C-15"},0)),
-_xlfn.VSTACK({"Customer","Sales"},_xlfn.HSTACK(_xlpm.su,_xlfn.MAP(_xlpm.su,_xlfn.LAMBDA(_xlpm.z,SUM(_xlfn._xlws.FILTER(D3:D36,_xlpm.zz=_xlpm.z))))))
-)</f>
-        <v>Customer</v>
-      </c>
-      <c r="G18" s="5" t="str">
-        <v>Sales</v>
-      </c>
-      <c r="I18" s="4" t="str" cm="1">
-        <f t="array" ref="I18:J26">_xlfn.LET(
 _xlpm.xmap,_xlfn.LAMBDA(_xlpm.v,_xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlpm.v,$F$3:$F$8,$G$3:$G$8,"NA"),IF(_xlpm.z="NA",_xlpm.v,Xref(_xlpm.z)))),
 _xlpm.nID,_xlfn.MAP(F3:F8,_xlfn.LAMBDA(_xlpm.z,IF(ISNUMBER(_xlfn.XMATCH(_xlpm.z,F3:F8)),_xlpm.xmap(_xlpm.z),_xlpm.z))),
 _xlpm.q,_xlfn.HSTACK($F$3:$F$8,_xlpm.nID),
@@ -3341,11 +3326,11 @@
 )</f>
         <v>Customer</v>
       </c>
-      <c r="J18" s="5" t="str">
+      <c r="G18" s="5" t="str">
         <v>Sales</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="11">
         <v>45212</v>
       </c>
@@ -3361,14 +3346,8 @@
       <c r="G19" s="7">
         <v>86</v>
       </c>
-      <c r="I19" s="6" t="str">
-        <v>C-3</v>
-      </c>
-      <c r="J19" s="7">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>45220</v>
       </c>
@@ -3384,14 +3363,8 @@
       <c r="G20" s="7">
         <v>11</v>
       </c>
-      <c r="I20" s="6" t="str">
-        <v>C-4</v>
-      </c>
-      <c r="J20" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>45222</v>
       </c>
@@ -3407,14 +3380,8 @@
       <c r="G21" s="9">
         <v>52</v>
       </c>
-      <c r="I21" s="6" t="str">
-        <v>C-8</v>
-      </c>
-      <c r="J21" s="9">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
         <v>45222</v>
       </c>
@@ -3430,14 +3397,8 @@
       <c r="G22" s="7">
         <v>92</v>
       </c>
-      <c r="I22" s="6" t="str">
-        <v>C-10</v>
-      </c>
-      <c r="J22" s="7">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
         <v>45239</v>
       </c>
@@ -3453,14 +3414,8 @@
       <c r="G23" s="7">
         <v>35</v>
       </c>
-      <c r="I23" s="6" t="str">
-        <v>C-11</v>
-      </c>
-      <c r="J23" s="7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <v>45240</v>
       </c>
@@ -3476,14 +3431,8 @@
       <c r="G24" s="7">
         <v>347</v>
       </c>
-      <c r="I24" s="6" t="str">
-        <v>C-13</v>
-      </c>
-      <c r="J24" s="7">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="11">
         <v>45246</v>
       </c>
@@ -3499,14 +3448,8 @@
       <c r="G25" s="7">
         <v>114</v>
       </c>
-      <c r="I25" s="6" t="str">
-        <v>C-14</v>
-      </c>
-      <c r="J25" s="7">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
         <v>45262</v>
       </c>
@@ -3522,14 +3465,8 @@
       <c r="G26" s="7">
         <v>85</v>
       </c>
-      <c r="I26" s="6" t="str">
-        <v>C-15</v>
-      </c>
-      <c r="J26" s="7">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="11">
         <v>45264</v>
       </c>
@@ -3540,7 +3477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
         <v>45276</v>
       </c>
@@ -3551,7 +3488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="11">
         <v>45284</v>
       </c>
@@ -3562,7 +3499,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="11">
         <v>45286</v>
       </c>
@@ -3573,7 +3510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="11">
         <v>45292</v>
       </c>
@@ -3584,7 +3521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="11">
         <v>45301</v>
       </c>

</xml_diff>